<commit_message>
6 initial configuration of DEC project
</commit_message>
<xml_diff>
--- a/FG_PrjDoc.xlsx
+++ b/FG_PrjDoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\FG9322\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\FG9326M8GTEI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549654BD-9F07-4A6F-9D4D-6E3FB2D0C41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BB06B9-2EFE-4949-A0C0-BFBA8FFFF009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="847" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="847" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Func" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <sheet name="ADCMUX" sheetId="5" r:id="rId8"/>
     <sheet name="Connector Mapping" sheetId="11" r:id="rId9"/>
     <sheet name="L1-L8" sheetId="12" r:id="rId10"/>
-    <sheet name="Func TBA" sheetId="10" r:id="rId11"/>
+    <sheet name="VehStateMachine" sheetId="16" r:id="rId11"/>
+    <sheet name="VO Data" sheetId="14" r:id="rId12"/>
+    <sheet name="Func TBA" sheetId="10" r:id="rId13"/>
+    <sheet name="Func DEC" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="579">
   <si>
     <t>Central Body Module</t>
   </si>
@@ -1493,6 +1496,341 @@
   </si>
   <si>
     <t>Update FBL according to new memory layout.</t>
+  </si>
+  <si>
+    <t>System re-programming</t>
+  </si>
+  <si>
+    <t>System enconding</t>
+  </si>
+  <si>
+    <t>VIN storing</t>
+  </si>
+  <si>
+    <t>Diagnosis control master</t>
+  </si>
+  <si>
+    <t>QC mode</t>
+  </si>
+  <si>
+    <t>CAN router</t>
+  </si>
+  <si>
+    <t>CAN master</t>
+  </si>
+  <si>
+    <t>Partial network control</t>
+  </si>
+  <si>
+    <t>Chassis data storing</t>
+  </si>
+  <si>
+    <t>Upholstery and paint storing</t>
+  </si>
+  <si>
+    <t>Vehicle order storing</t>
+  </si>
+  <si>
+    <t>Build date storing</t>
+  </si>
+  <si>
+    <t>SW Module</t>
+  </si>
+  <si>
+    <t>Vehicle state manager</t>
+  </si>
+  <si>
+    <t>Software-hardware version</t>
+  </si>
+  <si>
+    <t>System back-up</t>
+  </si>
+  <si>
+    <t>Supply state manager</t>
+  </si>
+  <si>
+    <t>In-Vehicle Error Notification</t>
+  </si>
+  <si>
+    <t>Electric powertrain motor control</t>
+  </si>
+  <si>
+    <t>Electric power steering motor control</t>
+  </si>
+  <si>
+    <t>Collision detection</t>
+  </si>
+  <si>
+    <t>Electric fan for EPS cooling</t>
+  </si>
+  <si>
+    <t>Temperature sensor for EPS</t>
+  </si>
+  <si>
+    <t>Speed sensor processing</t>
+  </si>
+  <si>
+    <t>RPM calculation of electric motor</t>
+  </si>
+  <si>
+    <t>Diagnostic messages buffer</t>
+  </si>
+  <si>
+    <t>CAN messages buffer</t>
+  </si>
+  <si>
+    <t>MCU safety measures</t>
+  </si>
+  <si>
+    <t>Drive-cycle control</t>
+  </si>
+  <si>
+    <t>Module names storing</t>
+  </si>
+  <si>
+    <t>CAN ISO-TP</t>
+  </si>
+  <si>
+    <t>Analog measurements for sensors</t>
+  </si>
+  <si>
+    <t>PWM signal generation for motors</t>
+  </si>
+  <si>
+    <t>E2E protection on ASIL messages</t>
+  </si>
+  <si>
+    <t>Multicore</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>DTC handling</t>
+  </si>
+  <si>
+    <t>NVM handling</t>
+  </si>
+  <si>
+    <t>CPU load calculation</t>
+  </si>
+  <si>
+    <t>5 series</t>
+  </si>
+  <si>
+    <t>3 series</t>
+  </si>
+  <si>
+    <t>4 series</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>WBADT534X2CE93000</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>WBAVB73558P102233</t>
+  </si>
+  <si>
+    <t>WBA3T3C50FP737967</t>
+  </si>
+  <si>
+    <t>Chassis number</t>
+  </si>
+  <si>
+    <t>G30</t>
+  </si>
+  <si>
+    <t>G26</t>
+  </si>
+  <si>
+    <t>8 series</t>
+  </si>
+  <si>
+    <t>F93</t>
+  </si>
+  <si>
+    <t>E46</t>
+  </si>
+  <si>
+    <t>Upholstery / paint</t>
+  </si>
+  <si>
+    <t>black / M8GTE</t>
+  </si>
+  <si>
+    <t>black / black sapphire</t>
+  </si>
+  <si>
+    <t>white / beige</t>
+  </si>
+  <si>
+    <t>grey / black sapphire</t>
+  </si>
+  <si>
+    <t>Software version</t>
+  </si>
+  <si>
+    <t>Hardware version</t>
+  </si>
+  <si>
+    <t>Calibration version</t>
+  </si>
+  <si>
+    <t>Coding version</t>
+  </si>
+  <si>
+    <t>Option list</t>
+  </si>
+  <si>
+    <t>Steer-by-wire
+Brake-by-wire
+Bluetooth control
+Remote ventilation
+Automatic climate control
+Windshield wiper normal speed
+Digital Cluster
+Reverse camera
+Collision assist
+Central locking
+Automatic lights
+Automatic wipers
+Automatic transmission / electric drivetrain
+Remote start
+5V electric drivetrain</t>
+  </si>
+  <si>
+    <t>Build date</t>
+  </si>
+  <si>
+    <t>01.05.2025</t>
+  </si>
+  <si>
+    <t>Module names</t>
+  </si>
+  <si>
+    <t>Central Body Module 1 - CBM1
+Digital Main Unit 1 - DMU1
+Power Distribution Module 1 - PDM1
+Drive Electronic Controller 1 - DEC1</t>
+  </si>
+  <si>
+    <t>1.1.1
+1.1.1
+1.1.1
+1.1.1</t>
+  </si>
+  <si>
+    <t>WBAEG2311MC291143</t>
+  </si>
+  <si>
+    <t>Vehicle states</t>
+  </si>
+  <si>
+    <t>Pre-conditions</t>
+  </si>
+  <si>
+    <t>Parked ignition off</t>
+  </si>
+  <si>
+    <t>Parked ignition on</t>
+  </si>
+  <si>
+    <t>Standing</t>
+  </si>
+  <si>
+    <t>Pre-drive-check</t>
+  </si>
+  <si>
+    <t>Driving</t>
+  </si>
+  <si>
+    <t>Post-drive-check</t>
+  </si>
+  <si>
+    <t>Vehicle error</t>
+  </si>
+  <si>
+    <t>Gearbox in park, central locking activated.</t>
+  </si>
+  <si>
+    <t>Gearbox in park, central locking de-activated.</t>
+  </si>
+  <si>
+    <t>Gearbox in drive or in park, ignition switched to position two.</t>
+  </si>
+  <si>
+    <t>Gearbox in drive and vehicle speed greater than zero.</t>
+  </si>
+  <si>
+    <t>In-Vehicle error preventing safe driving.</t>
+  </si>
+  <si>
+    <t>Additional state for checks</t>
+  </si>
+  <si>
+    <t>FBL</t>
+  </si>
+  <si>
+    <t>EncCal</t>
+  </si>
+  <si>
+    <t>ConfigMgr</t>
+  </si>
+  <si>
+    <t>VehState</t>
+  </si>
+  <si>
+    <t>EnergyManagement</t>
+  </si>
+  <si>
+    <t>IVEN</t>
+  </si>
+  <si>
+    <t>EPSControl</t>
+  </si>
+  <si>
+    <t>EMotorControl</t>
+  </si>
+  <si>
+    <t>ComMgr</t>
+  </si>
+  <si>
+    <t>SysMgr</t>
+  </si>
+  <si>
+    <t>DiagMaster</t>
+  </si>
+  <si>
+    <t>ComMaster</t>
+  </si>
+  <si>
+    <t>ColDet</t>
+  </si>
+  <si>
+    <t>DcyHandler</t>
+  </si>
+  <si>
+    <t>McuSm</t>
+  </si>
+  <si>
+    <t>Ain</t>
+  </si>
+  <si>
+    <t>Pwm</t>
+  </si>
+  <si>
+    <t>FreeRTOS</t>
+  </si>
+  <si>
+    <t>Dem</t>
+  </si>
+  <si>
+    <t>Nvm</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1902,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1703,6 +2041,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -1784,7 +2134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1939,6 +2289,21 @@
     <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7409,6 +7774,300 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBF02F53-59A5-454C-A300-F860A5996AFF}">
+  <dimension ref="D4:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D4" s="65" t="s">
+        <v>544</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="64" t="s">
+        <v>546</v>
+      </c>
+      <c r="E5" s="64" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="64" t="s">
+        <v>547</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="64" t="s">
+        <v>548</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="64" t="s">
+        <v>549</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9" s="64" t="s">
+        <v>550</v>
+      </c>
+      <c r="E9" s="64" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="64" t="s">
+        <v>552</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="64" t="s">
+        <v>551</v>
+      </c>
+      <c r="E11" s="64" t="s">
+        <v>558</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3DD87A-5819-466C-8F24-99C8AF7DD494}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="66" t="s">
+        <v>518</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>524</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>513</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>515</v>
+      </c>
+      <c r="E1" s="67" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="66" t="s">
+        <v>516</v>
+      </c>
+      <c r="B2" s="70" t="s">
+        <v>543</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>517</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>520</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="66" t="s">
+        <v>521</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>525</v>
+      </c>
+      <c r="C3" s="67" t="s">
+        <v>522</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>523</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="66" t="s">
+        <v>527</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>528</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>529</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>530</v>
+      </c>
+      <c r="E4" s="70" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="66" t="s">
+        <v>532</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>542</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>542</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>542</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="66" t="s">
+        <v>533</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>542</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>542</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>542</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="66" t="s">
+        <v>534</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>542</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>542</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>542</v>
+      </c>
+      <c r="E7" s="68" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="66" t="s">
+        <v>535</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>542</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>542</v>
+      </c>
+      <c r="E8" s="71" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="225.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="66" t="s">
+        <v>536</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>537</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>537</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>537</v>
+      </c>
+      <c r="E9" s="69" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="66" t="s">
+        <v>538</v>
+      </c>
+      <c r="B10" s="72" t="s">
+        <v>539</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>539</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>539</v>
+      </c>
+      <c r="E10" s="72" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="66" t="s">
+        <v>540</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>541</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>541</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>541</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>541</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B876571-A643-4A6E-AEEF-90DA4EBD900F}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
@@ -7574,6 +8233,345 @@
       </c>
       <c r="C14" s="63" t="s">
         <v>473</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED723F3-1E1E-412C-8F3F-6D02F8585AB8}">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B5" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>479</v>
+      </c>
+      <c r="B6" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>477</v>
+      </c>
+      <c r="B7" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>478</v>
+      </c>
+      <c r="B8" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>480</v>
+      </c>
+      <c r="B9" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>481</v>
+      </c>
+      <c r="B10" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>482</v>
+      </c>
+      <c r="B11" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>483</v>
+      </c>
+      <c r="B12" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>484</v>
+      </c>
+      <c r="B13" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>485</v>
+      </c>
+      <c r="B14" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>487</v>
+      </c>
+      <c r="B15" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>488</v>
+      </c>
+      <c r="B16" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>489</v>
+      </c>
+      <c r="B17" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>490</v>
+      </c>
+      <c r="B18" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>491</v>
+      </c>
+      <c r="B19" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>492</v>
+      </c>
+      <c r="B20" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>493</v>
+      </c>
+      <c r="B21" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>494</v>
+      </c>
+      <c r="B22" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>495</v>
+      </c>
+      <c r="B23" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>496</v>
+      </c>
+      <c r="B24" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>497</v>
+      </c>
+      <c r="B25" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>498</v>
+      </c>
+      <c r="B26" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>500</v>
+      </c>
+      <c r="B27" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>499</v>
+      </c>
+      <c r="B28" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>501</v>
+      </c>
+      <c r="B29" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>502</v>
+      </c>
+      <c r="B30" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>503</v>
+      </c>
+      <c r="B31" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>504</v>
+      </c>
+      <c r="B32" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>505</v>
+      </c>
+      <c r="B33" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>506</v>
+      </c>
+      <c r="B34" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>507</v>
+      </c>
+      <c r="B35" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>508</v>
+      </c>
+      <c r="B36" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>512</v>
+      </c>
+      <c r="B37" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>509</v>
+      </c>
+      <c r="B38" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>510</v>
+      </c>
+      <c r="B39" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>511</v>
+      </c>
+      <c r="B40" t="s">
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -17700,8 +18698,8 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
7 Integration of Aurix Code Examples
</commit_message>
<xml_diff>
--- a/FG_PrjDoc.xlsx
+++ b/FG_PrjDoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\FG9326M8GTEI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BB06B9-2EFE-4949-A0C0-BFBA8FFFF009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFD6413-3801-4B18-8989-5F9005A79E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="847" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="847" firstSheet="8" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Func" sheetId="2" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="VO Data" sheetId="14" r:id="rId12"/>
     <sheet name="Func TBA" sheetId="10" r:id="rId13"/>
     <sheet name="Func DEC" sheetId="13" r:id="rId14"/>
+    <sheet name="Modules-todo-DEC" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -8244,7 +8245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED723F3-1E1E-412C-8F3F-6D02F8585AB8}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -8575,6 +8576,18 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B87DE9-AC8C-4975-9461-2DE4464EA131}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
7 Following modules are done: ColDet, DcyHandler, EncCal, EnergyMgmt, Iven, Can, Ain, Dma, Eru, Gtm, Irq, Fls, Nvm, Crc, McuSm, Os, Smu, SysMgr, Wdg, SCR | Following topics are done: System encoding, calibration handling, VO Data handling (VIN, chassis data, upholstery paint, vehicle order storing, build date storing, software-hardware version, module name, QC mode, Supply state manager, drive-cycle control, vehicle state manager, in-vehicle error notification, MCU safety measures, collision detections, multi core, os, NVM handling, E2E, CAN buffer
</commit_message>
<xml_diff>
--- a/FG_PrjDoc.xlsx
+++ b/FG_PrjDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\FG9326M8GTEI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0B2477-09F3-499D-85A4-B2EBBF28840D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90EDA2F-0153-4A8D-8C50-4CDF4ED44850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="847" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="847" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Func" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="584">
   <si>
     <t>Central Body Module</t>
   </si>
@@ -1712,9 +1712,6 @@
     <t>EncCal</t>
   </si>
   <si>
-    <t>VehState</t>
-  </si>
-  <si>
     <t>EnergyManagement</t>
   </si>
   <si>
@@ -1848,9 +1845,6 @@
   </si>
   <si>
     <t>Additional state for checks.</t>
-  </si>
-  <si>
-    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2330,7 +2324,6 @@
     <xf numFmtId="0" fontId="1" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -7658,8 +7651,8 @@
   </sheetPr>
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7671,10 +7664,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
+        <v>558</v>
+      </c>
+      <c r="B1" s="73" t="s">
         <v>559</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>560</v>
       </c>
       <c r="D1" s="74" t="s">
         <v>233</v>
@@ -7685,10 +7678,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B2" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D2" t="s">
         <v>455</v>
@@ -7699,10 +7692,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B3" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D3" s="71" t="s">
         <v>456</v>
@@ -7713,10 +7706,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D4" s="71" t="s">
         <v>16</v>
@@ -7727,10 +7720,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D5" s="71" t="s">
         <v>457</v>
@@ -7741,30 +7734,30 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="72" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D6" t="s">
         <v>458</v>
       </c>
       <c r="E6" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="72" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B7" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D7" s="71" t="s">
         <v>459</v>
       </c>
       <c r="E7" s="71" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -7772,35 +7765,35 @@
         <v>538</v>
       </c>
       <c r="B8" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D8" t="s">
         <v>460</v>
       </c>
       <c r="E8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B9" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D9" t="s">
         <v>461</v>
       </c>
       <c r="E9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="72" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B10" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D10" s="71" t="s">
         <v>462</v>
@@ -7811,10 +7804,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="72" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B11" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D11" s="71" t="s">
         <v>463</v>
@@ -7825,10 +7818,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="72" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B12" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D12" s="71" t="s">
         <v>464</v>
@@ -7839,10 +7832,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="72" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B13" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D13" s="71" t="s">
         <v>465</v>
@@ -7853,24 +7846,24 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="72" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B14" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D14" s="71" t="s">
         <v>467</v>
       </c>
       <c r="E14" s="71" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="72" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B15" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D15" s="71" t="s">
         <v>468</v>
@@ -7881,10 +7874,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="72" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B16" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D16" t="s">
         <v>469</v>
@@ -7895,184 +7888,184 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D17" s="71" t="s">
         <v>470</v>
       </c>
       <c r="E17" s="71" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="72" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B18" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D18" s="71" t="s">
         <v>471</v>
       </c>
       <c r="E18" s="71" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="72" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D19" t="s">
         <v>472</v>
       </c>
       <c r="E19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="72" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D20" t="s">
         <v>473</v>
       </c>
       <c r="E20" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="72" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B21" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D21" s="71" t="s">
         <v>474</v>
       </c>
       <c r="E21" s="71" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="72" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D22" t="s">
         <v>475</v>
       </c>
       <c r="E22" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="72" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D23" t="s">
         <v>476</v>
       </c>
       <c r="E23" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="72" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B24" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D24" t="s">
         <v>477</v>
       </c>
       <c r="E24" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="72" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B25" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D25" t="s">
         <v>478</v>
       </c>
       <c r="E25" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="72" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B26" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D26" s="71" t="s">
         <v>480</v>
       </c>
       <c r="E26" s="71" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D27" t="s">
         <v>479</v>
       </c>
       <c r="E27" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="72" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B28" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D28" s="71" t="s">
         <v>481</v>
       </c>
       <c r="E28" s="71" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="72" t="s">
-        <v>579</v>
-      </c>
-      <c r="B29" s="77" t="s">
-        <v>585</v>
+        <v>578</v>
+      </c>
+      <c r="B29" s="75" t="s">
+        <v>580</v>
       </c>
       <c r="D29" s="71" t="s">
         <v>482</v>
       </c>
       <c r="E29" s="71" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -8080,7 +8073,7 @@
         <v>537</v>
       </c>
       <c r="B30" s="76" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D30" s="71" t="s">
         <v>483</v>
@@ -8090,11 +8083,11 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D31" s="78" t="s">
+      <c r="D31" s="77" t="s">
         <v>484</v>
       </c>
-      <c r="E31" s="78" t="s">
-        <v>565</v>
+      <c r="E31" s="77" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -8102,7 +8095,7 @@
         <v>485</v>
       </c>
       <c r="E32" s="71" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
@@ -8110,7 +8103,7 @@
         <v>486</v>
       </c>
       <c r="E33" s="71" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
@@ -8118,7 +8111,7 @@
         <v>487</v>
       </c>
       <c r="E34" s="71" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
@@ -8126,7 +8119,7 @@
         <v>488</v>
       </c>
       <c r="E35" s="71" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
@@ -8134,7 +8127,7 @@
         <v>489</v>
       </c>
       <c r="E36" s="71" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
@@ -8142,7 +8135,7 @@
         <v>490</v>
       </c>
       <c r="E37" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
@@ -8150,7 +8143,7 @@
         <v>491</v>
       </c>
       <c r="E38" s="71" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -8293,7 +8286,7 @@
         <v>528</v>
       </c>
       <c r="I5" s="60" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -8362,7 +8355,7 @@
         <v>530</v>
       </c>
       <c r="I8" s="60" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -8382,10 +8375,10 @@
         <v>286</v>
       </c>
       <c r="H9" s="60" t="s">
+        <v>581</v>
+      </c>
+      <c r="I9" s="60" t="s">
         <v>582</v>
-      </c>
-      <c r="I9" s="60" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -10124,7 +10117,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
@@ -19785,7 +19778,7 @@
         <v>498</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -19805,7 +19798,7 @@
         <v>505</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
@@ -19825,7 +19818,7 @@
         <v>510</v>
       </c>
       <c r="F4" s="66" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60.75" x14ac:dyDescent="0.3">
@@ -19948,7 +19941,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="285.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A11" s="62" t="s">
         <v>519</v>
       </c>

</xml_diff>

<commit_message>
23 Final commit ... I hope
</commit_message>
<xml_diff>
--- a/FG_PrjDoc.xlsx
+++ b/FG_PrjDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\FG9326M8GTEI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8AF4F0-5A59-4B9C-8EEB-B64D18AD0A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE6C377-A2F9-4F2D-8B23-F6FC2BF6642C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="847" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="847" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Func" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="252">
   <si>
     <t>Central Body Module</t>
   </si>
@@ -627,15 +627,6 @@
     <t>CLIMA FAN SUPPLY</t>
   </si>
   <si>
-    <t>5 series</t>
-  </si>
-  <si>
-    <t>3 series</t>
-  </si>
-  <si>
-    <t>4 series</t>
-  </si>
-  <si>
     <t>VIN</t>
   </si>
   <si>
@@ -660,9 +651,6 @@
     <t>G26</t>
   </si>
   <si>
-    <t>8 series</t>
-  </si>
-  <si>
     <t>F93</t>
   </si>
   <si>
@@ -672,18 +660,6 @@
     <t>Upholstery / paint</t>
   </si>
   <si>
-    <t>black / M8GTE</t>
-  </si>
-  <si>
-    <t>black / black sapphire</t>
-  </si>
-  <si>
-    <t>white / beige</t>
-  </si>
-  <si>
-    <t>grey / black sapphire</t>
-  </si>
-  <si>
     <t>Software version</t>
   </si>
   <si>
@@ -702,18 +678,9 @@
     <t>Build date</t>
   </si>
   <si>
-    <t>01.05.2025</t>
-  </si>
-  <si>
     <t>Module names</t>
   </si>
   <si>
-    <t>1.1.1
-1.1.1
-1.1.1
-1.1.1</t>
-  </si>
-  <si>
     <t>WBAEG2311MC291143</t>
   </si>
   <si>
@@ -759,9 +726,6 @@
     <t>E39</t>
   </si>
   <si>
-    <t>black / metallic grey</t>
-  </si>
-  <si>
     <t>WBADT42040CX97550</t>
   </si>
   <si>
@@ -777,31 +741,6 @@
     <t>Diagnostic Mode Activated</t>
   </si>
   <si>
-    <t>Central Body Module 1 - CBM1
-Digital Main Unit 1 - DMU1
-Drive Electronic Controller 1 - DEC1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Bluetooth control
-Remote ventilation
-Automatic climate control
-Windshield wiper normal speed
-Digital Cluster
-Reverse camera
-Collision assist
-Central locking
-Automatic lights
-Automatic wipers
-Remote start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1.1
-1.1.1
-1.1.1
-</t>
-  </si>
-  <si>
     <t>Digital Cluster Error</t>
   </si>
   <si>
@@ -827,6 +766,36 @@
   </si>
   <si>
     <t>MCU Safety Measures</t>
+  </si>
+  <si>
+    <t>P010525</t>
+  </si>
+  <si>
+    <t>CBM1
+DMU1
+DEC1</t>
+  </si>
+  <si>
+    <t>111
+111
+111</t>
+  </si>
+  <si>
+    <t>BTC
+RVENT
+CLIMA
+DIGCLS
+REVCAM
+COLLASSIST
+CENLOC
+AL
+AW</t>
+  </si>
+  <si>
+    <t>A83475</t>
+  </si>
+  <si>
+    <t>416A62</t>
   </si>
 </sst>
 </file>
@@ -996,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1033,7 +1002,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1045,7 +1013,6 @@
     <xf numFmtId="14" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1055,6 +1022,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1341,7 +1318,7 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -1382,7 +1359,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,7 +1370,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1415,7 +1392,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,7 +1403,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1478,10 +1455,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1490,7 +1467,7 @@
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,10 +1545,10 @@
         <v>28</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1588,10 +1565,10 @@
         <v>90</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1608,10 +1585,10 @@
         <v>91</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1628,10 +1605,10 @@
         <v>92</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1648,10 +1625,10 @@
         <v>93</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1668,10 +1645,10 @@
         <v>94</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1688,10 +1665,10 @@
         <v>95</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1708,10 +1685,10 @@
         <v>96</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1925,7 +1902,7 @@
         <v>41</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1945,7 +1922,7 @@
         <v>98</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1965,7 +1942,7 @@
         <v>99</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2129,19 +2106,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="23" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2152,13 +2129,13 @@
       <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="24" t="s">
         <v>163</v>
       </c>
       <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2167,13 +2144,13 @@
       <c r="B3" s="7">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="24" t="s">
         <v>166</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2182,13 +2159,13 @@
       <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>167</v>
       </c>
       <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2197,13 +2174,13 @@
       <c r="B5" s="7">
         <v>4</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>164</v>
       </c>
       <c r="E5" s="7">
         <v>3</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="26" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2212,13 +2189,13 @@
       <c r="B6" s="7">
         <v>5</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="24" t="s">
         <v>168</v>
       </c>
       <c r="E6" s="7">
         <v>4</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="26" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2227,13 +2204,13 @@
       <c r="B7" s="7">
         <v>6</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="24" t="s">
         <v>169</v>
       </c>
       <c r="E7" s="7">
         <v>5</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2242,13 +2219,13 @@
       <c r="B8" s="7">
         <v>7</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>172</v>
       </c>
       <c r="E8" s="7">
         <v>6</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2257,13 +2234,13 @@
       <c r="B9" s="7">
         <v>8</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="24" t="s">
         <v>165</v>
       </c>
       <c r="E9" s="7">
         <v>7</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="26" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2272,13 +2249,13 @@
       <c r="B10" s="7">
         <v>9</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="24" t="s">
         <v>170</v>
       </c>
       <c r="E10" s="7">
         <v>8</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="26" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2287,13 +2264,13 @@
       <c r="B11" s="7">
         <v>10</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="24" t="s">
         <v>171</v>
       </c>
       <c r="E11" s="7">
         <v>9</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="26" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2304,13 +2281,13 @@
       <c r="B12" s="7">
         <v>1</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>173</v>
       </c>
       <c r="E12" s="7">
         <v>10</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2319,13 +2296,13 @@
       <c r="B13" s="7">
         <v>2</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>174</v>
       </c>
       <c r="E13" s="7">
         <v>11</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2334,13 +2311,13 @@
       <c r="B14" s="7">
         <v>3</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="24" t="s">
         <v>175</v>
       </c>
       <c r="E14" s="7">
         <v>12</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2349,13 +2326,13 @@
       <c r="B15" s="7">
         <v>4</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="24" t="s">
         <v>176</v>
       </c>
       <c r="E15" s="7">
         <v>13</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2364,13 +2341,13 @@
       <c r="B16" s="7">
         <v>5</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="24" t="s">
         <v>177</v>
       </c>
       <c r="E16" s="7">
         <v>14</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2379,13 +2356,13 @@
       <c r="B17" s="7">
         <v>6</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="24" t="s">
         <v>178</v>
       </c>
       <c r="E17" s="7">
         <v>15</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="25" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2394,7 +2371,7 @@
       <c r="B18" s="7">
         <v>7</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2403,7 +2380,7 @@
       <c r="B19" s="7">
         <v>8</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2412,7 +2389,7 @@
       <c r="B20" s="7">
         <v>9</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2421,7 +2398,7 @@
       <c r="B21" s="7">
         <v>10</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2432,7 +2409,7 @@
       <c r="B22" s="7">
         <v>1</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="24" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2441,7 +2418,7 @@
       <c r="B23" s="7">
         <v>2</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="24" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2450,7 +2427,7 @@
       <c r="B24" s="7">
         <v>3</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="24" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2459,7 +2436,7 @@
       <c r="B25" s="7">
         <v>4</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="24" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2468,7 +2445,7 @@
       <c r="B26" s="7">
         <v>5</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="24" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2477,7 +2454,7 @@
       <c r="B27" s="7">
         <v>6</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="24" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2486,7 +2463,7 @@
       <c r="B28" s="7">
         <v>7</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2495,7 +2472,7 @@
       <c r="B29" s="7">
         <v>8</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="24" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2504,7 +2481,7 @@
       <c r="B30" s="7">
         <v>9</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="24" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2513,7 +2490,7 @@
       <c r="B31" s="7">
         <v>10</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="24" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2524,7 +2501,7 @@
       <c r="B32" s="7">
         <v>1</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="24" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2533,7 +2510,7 @@
       <c r="B33" s="7">
         <v>2</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="24" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2542,7 +2519,7 @@
       <c r="B34" s="7">
         <v>3</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="24" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2551,7 +2528,7 @@
       <c r="B35" s="7">
         <v>4</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2560,7 +2537,7 @@
       <c r="B36" s="7">
         <v>5</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2569,7 +2546,7 @@
       <c r="B37" s="7">
         <v>6</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2578,7 +2555,7 @@
       <c r="B38" s="7">
         <v>7</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2587,7 +2564,7 @@
       <c r="B39" s="7">
         <v>8</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2596,7 +2573,7 @@
       <c r="B40" s="7">
         <v>9</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2605,7 +2582,7 @@
       <c r="B41" s="7">
         <v>10</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2616,7 +2593,7 @@
       <c r="B42" s="7">
         <v>1</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="24" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2625,7 +2602,7 @@
       <c r="B43" s="7">
         <v>2</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="24" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2634,7 +2611,7 @@
       <c r="B44" s="7">
         <v>3</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="24" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2643,7 +2620,7 @@
       <c r="B45" s="7">
         <v>4</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="24" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2652,7 +2629,7 @@
       <c r="B46" s="7">
         <v>5</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="24" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2661,7 +2638,7 @@
       <c r="B47" s="7">
         <v>6</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="24" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2670,7 +2647,7 @@
       <c r="B48" s="7">
         <v>7</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="24" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2679,7 +2656,7 @@
       <c r="B49" s="7">
         <v>8</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="24" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2688,7 +2665,7 @@
       <c r="B50" s="7">
         <v>9</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="24" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2697,7 +2674,7 @@
       <c r="B51" s="7">
         <v>10</v>
       </c>
-      <c r="C51" s="27" t="s">
+      <c r="C51" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2708,7 +2685,7 @@
       <c r="B52" s="7">
         <v>1</v>
       </c>
-      <c r="C52" s="26" t="s">
+      <c r="C52" s="24" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2717,7 +2694,7 @@
       <c r="B53" s="7">
         <v>2</v>
       </c>
-      <c r="C53" s="26" t="s">
+      <c r="C53" s="24" t="s">
         <v>195</v>
       </c>
     </row>
@@ -2726,7 +2703,7 @@
       <c r="B54" s="7">
         <v>3</v>
       </c>
-      <c r="C54" s="26" t="s">
+      <c r="C54" s="24" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2735,7 +2712,7 @@
       <c r="B55" s="7">
         <v>4</v>
       </c>
-      <c r="C55" s="27" t="s">
+      <c r="C55" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2744,7 +2721,7 @@
       <c r="B56" s="7">
         <v>5</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2753,7 +2730,7 @@
       <c r="B57" s="7">
         <v>6</v>
       </c>
-      <c r="C57" s="27" t="s">
+      <c r="C57" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2762,7 +2739,7 @@
       <c r="B58" s="7">
         <v>7</v>
       </c>
-      <c r="C58" s="27" t="s">
+      <c r="C58" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2771,7 +2748,7 @@
       <c r="B59" s="7">
         <v>8</v>
       </c>
-      <c r="C59" s="27" t="s">
+      <c r="C59" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2780,7 +2757,7 @@
       <c r="B60" s="7">
         <v>9</v>
       </c>
-      <c r="C60" s="27" t="s">
+      <c r="C60" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2789,7 +2766,7 @@
       <c r="B61" s="7">
         <v>10</v>
       </c>
-      <c r="C61" s="27" t="s">
+      <c r="C61" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2800,7 +2777,7 @@
       <c r="B62" s="7">
         <v>1</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="C62" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2809,7 +2786,7 @@
       <c r="B63" s="7">
         <v>2</v>
       </c>
-      <c r="C63" s="27" t="s">
+      <c r="C63" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2818,7 +2795,7 @@
       <c r="B64" s="7">
         <v>3</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="C64" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2827,7 +2804,7 @@
       <c r="B65" s="7">
         <v>4</v>
       </c>
-      <c r="C65" s="27" t="s">
+      <c r="C65" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2836,7 +2813,7 @@
       <c r="B66" s="7">
         <v>5</v>
       </c>
-      <c r="C66" s="27" t="s">
+      <c r="C66" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2845,7 +2822,7 @@
       <c r="B67" s="7">
         <v>6</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C67" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2854,7 +2831,7 @@
       <c r="B68" s="7">
         <v>7</v>
       </c>
-      <c r="C68" s="27" t="s">
+      <c r="C68" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2863,7 +2840,7 @@
       <c r="B69" s="7">
         <v>8</v>
       </c>
-      <c r="C69" s="27" t="s">
+      <c r="C69" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2872,7 +2849,7 @@
       <c r="B70" s="7">
         <v>9</v>
       </c>
-      <c r="C70" s="27" t="s">
+      <c r="C70" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2881,7 +2858,7 @@
       <c r="B71" s="7">
         <v>10</v>
       </c>
-      <c r="C71" s="27" t="s">
+      <c r="C71" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2892,7 +2869,7 @@
       <c r="B72" s="7">
         <v>1</v>
       </c>
-      <c r="C72" s="26" t="s">
+      <c r="C72" s="24" t="s">
         <v>197</v>
       </c>
     </row>
@@ -2901,7 +2878,7 @@
       <c r="B73" s="7">
         <v>2</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="C73" s="24" t="s">
         <v>198</v>
       </c>
     </row>
@@ -2910,7 +2887,7 @@
       <c r="B74" s="7">
         <v>3</v>
       </c>
-      <c r="C74" s="27" t="s">
+      <c r="C74" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2919,7 +2896,7 @@
       <c r="B75" s="7">
         <v>4</v>
       </c>
-      <c r="C75" s="27" t="s">
+      <c r="C75" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2928,7 +2905,7 @@
       <c r="B76" s="7">
         <v>5</v>
       </c>
-      <c r="C76" s="27" t="s">
+      <c r="C76" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2937,7 +2914,7 @@
       <c r="B77" s="7">
         <v>6</v>
       </c>
-      <c r="C77" s="27" t="s">
+      <c r="C77" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2946,7 +2923,7 @@
       <c r="B78" s="7">
         <v>7</v>
       </c>
-      <c r="C78" s="27" t="s">
+      <c r="C78" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2955,7 +2932,7 @@
       <c r="B79" s="7">
         <v>8</v>
       </c>
-      <c r="C79" s="27" t="s">
+      <c r="C79" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2964,7 +2941,7 @@
       <c r="B80" s="7">
         <v>9</v>
       </c>
-      <c r="C80" s="27" t="s">
+      <c r="C80" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2973,7 +2950,7 @@
       <c r="B81" s="7">
         <v>10</v>
       </c>
-      <c r="C81" s="27" t="s">
+      <c r="C81" s="25" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2991,10 +2968,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3005,223 +2982,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="28">
+        <v>8</v>
+      </c>
+      <c r="C1" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1" s="28">
+        <v>4</v>
+      </c>
+      <c r="E1" s="28">
+        <v>3</v>
+      </c>
+      <c r="F1" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B3" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" s="30">
+        <v>475999</v>
+      </c>
+      <c r="C4" s="30">
+        <v>416475</v>
+      </c>
+      <c r="D4" s="30">
+        <v>300850</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" s="19" t="s">
+      <c r="B5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="E3" s="19" t="s">
+      <c r="B6" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="B7" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B8" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="135.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="B9" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="B10" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="60.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="180.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>248</v>
+      <c r="B11" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3532,13 +3509,21 @@
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="1">
+      <c r="D30" s="1"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="1">
         <v>5</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F31" s="10" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>